<commit_message>
Re-implement uncaught et unknown cobblemons list
</commit_message>
<xml_diff>
--- a/cobblemon_module/output.xlsx
+++ b/cobblemon_module/output.xlsx
@@ -1773,7 +1773,7 @@
       <c r="A14" s="78" t="n"/>
       <c r="B14" s="101" t="inlineStr">
         <is>
-          <t>Dernière update le 25.02.25 à 02:00</t>
+          <t>Dernière update le 25.02.25 à 02:26</t>
         </is>
       </c>
       <c r="Q14" s="78" t="n"/>
@@ -2590,7 +2590,7 @@
       <c r="A14" s="103" t="n"/>
       <c r="B14" s="124" t="inlineStr">
         <is>
-          <t>Dernière update le 25.02.25 à 02:00</t>
+          <t>Dernière update le 25.02.25 à 02:26</t>
         </is>
       </c>
       <c r="Q14" s="103" t="n"/>
@@ -3415,7 +3415,7 @@
       <c r="A14" s="126" t="n"/>
       <c r="B14" s="150" t="inlineStr">
         <is>
-          <t>Dernière update le 25.02.25 à 02:00</t>
+          <t>Dernière update le 25.02.25 à 02:26</t>
         </is>
       </c>
       <c r="Q14" s="126" t="n"/>

</xml_diff>